<commit_message>
changed spread sheet with a few new values
</commit_message>
<xml_diff>
--- a/Ozone 2018 Auton Measurements.xlsx
+++ b/Ozone 2018 Auton Measurements.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18460" windowHeight="5690" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RRSwRScLLSwLSc" sheetId="1" r:id="rId1"/>
@@ -20,6 +15,7 @@
     <sheet name="CRSwCLSw" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:G19"/>
 </workbook>
 </file>
 
@@ -325,7 +321,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -697,7 +693,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1159,13 +1155,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1531,10 +1529,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1775,7 +1773,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2031,10 +2029,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -2426,7 +2424,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>